<commit_message>
new version that correct the name of service
</commit_message>
<xml_diff>
--- a/cqrs_pattern_flow_rules.xlsx
+++ b/cqrs_pattern_flow_rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huicha/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81500577-1E2B-7445-B8A6-7479BFA6FF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DF09FB-8F36-A94B-B817-05BD9B1ECD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="2800" windowWidth="27240" windowHeight="16440" xr2:uid="{6A876A9D-82A5-4A4C-94D8-56358ACF9BE0}"/>
   </bookViews>
@@ -52,7 +52,7 @@
     <t>COMMAND</t>
   </si>
   <si>
-    <t>ResolveActionAndPrincing</t>
+    <t>ResolveActionAndPricing</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>